<commit_message>
Completed Visual login section; updated links; finishedfooter
</commit_message>
<xml_diff>
--- a/Project Management/Project_Burndown_Chart.xlsx
+++ b/Project Management/Project_Burndown_Chart.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t>Designed, Created and Installed Site Logo</t>
+  </si>
+  <si>
+    <t>Login Section</t>
+  </si>
+  <si>
+    <t>Starting the Modal login</t>
+  </si>
+  <si>
+    <t>T05</t>
+  </si>
+  <si>
+    <t>T04</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Establishing correct links on home page</t>
+  </si>
+  <si>
+    <t>9/05.2017</t>
+  </si>
+  <si>
+    <t>Completed Modal Login section without DB</t>
   </si>
 </sst>
 </file>
@@ -1254,97 +1278,97 @@
                   <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>169</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>169</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,11 +1384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="322518992"/>
-        <c:axId val="322520168"/>
+        <c:axId val="321654504"/>
+        <c:axId val="321655680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="322518992"/>
+        <c:axId val="321654504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322520168"/>
+        <c:crossAx val="321655680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1477,7 +1501,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="322520168"/>
+        <c:axId val="321655680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322518992"/>
+        <c:crossAx val="321654504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2526,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,11 +3310,11 @@
         <v>3.4285714285714284</v>
       </c>
       <c r="G28" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -3313,11 +3337,11 @@
         <v>3.4285714285714284</v>
       </c>
       <c r="G29" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H29" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -3347,7 +3371,7 @@
       </c>
       <c r="H30" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -3374,7 +3398,7 @@
       </c>
       <c r="H31" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3401,7 +3425,7 @@
       </c>
       <c r="H32" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -3428,7 +3452,7 @@
       </c>
       <c r="H33" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -3455,7 +3479,7 @@
       </c>
       <c r="H34" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -3482,7 +3506,7 @@
       </c>
       <c r="H35" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -3509,7 +3533,7 @@
       </c>
       <c r="H36" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3539,7 +3563,7 @@
       </c>
       <c r="H37" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3566,7 +3590,7 @@
       </c>
       <c r="H38" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -3593,7 +3617,7 @@
       </c>
       <c r="H39" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -3620,7 +3644,7 @@
       </c>
       <c r="H40" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -3647,7 +3671,7 @@
       </c>
       <c r="H41" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -3674,7 +3698,7 @@
       </c>
       <c r="H42" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -3701,7 +3725,7 @@
       </c>
       <c r="H43" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -3731,7 +3755,7 @@
       </c>
       <c r="H44" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -3758,7 +3782,7 @@
       </c>
       <c r="H45" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -3785,7 +3809,7 @@
       </c>
       <c r="H46" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -3812,7 +3836,7 @@
       </c>
       <c r="H47" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -3839,7 +3863,7 @@
       </c>
       <c r="H48" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -3866,7 +3890,7 @@
       </c>
       <c r="H49" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -3893,7 +3917,7 @@
       </c>
       <c r="H50" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -3923,7 +3947,7 @@
       </c>
       <c r="H51" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -3950,7 +3974,7 @@
       </c>
       <c r="H52" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -3977,7 +4001,7 @@
       </c>
       <c r="H53" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -4004,7 +4028,7 @@
       </c>
       <c r="H54" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -4031,7 +4055,7 @@
       </c>
       <c r="H55" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -4058,7 +4082,7 @@
       </c>
       <c r="H56" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -4085,7 +4109,7 @@
       </c>
       <c r="H57" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -4114,13 +4138,13 @@
       </c>
       <c r="H58" s="11">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G59" s="11">
         <f>SUM(G2:G58)</f>
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4134,7 +4158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4230,7 +4256,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
-        <v>42800</v>
+        <v>42861</v>
       </c>
       <c r="B5" s="15">
         <v>3</v>
@@ -4250,7 +4276,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
-        <v>42800</v>
+        <v>42861</v>
       </c>
       <c r="B6" s="15">
         <v>3</v>
@@ -4269,28 +4295,64 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="18"/>
+      <c r="A7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
+      <c r="A8" s="14">
+        <v>42865</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="14">
+        <v>42865</v>
+      </c>
+      <c r="B9" s="15">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>

</xml_diff>